<commit_message>
First Use of chatGPT to add Kalman filter
</commit_message>
<xml_diff>
--- a/WaterDiag.xlsx
+++ b/WaterDiag.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dub/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dub/Code/MilanoWaterProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13B607E-7A03-D24B-8160-78475AB21152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CACAC79-D3AA-FB4B-985F-C1B893443012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18100" yWindow="500" windowWidth="31380" windowHeight="19020" xr2:uid="{60223CC9-929C-2C40-9DF4-4D5E66E85102}"/>
+    <workbookView xWindow="15080" yWindow="2200" windowWidth="31380" windowHeight="19020" xr2:uid="{60223CC9-929C-2C40-9DF4-4D5E66E85102}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="241">
   <si>
     <t>/*</t>
   </si>
@@ -48,9 +48,6 @@
     <t xml:space="preserve">*/ </t>
   </si>
   <si>
-    <t>/* CLIENTID</t>
-  </si>
-  <si>
     <t xml:space="preserve"> CH1 Unused Damaged/Dead</t>
   </si>
   <si>
@@ -315,9 +312,6 @@
     <t>House Water Pressure Value</t>
   </si>
   <si>
-    <t>* payload 0</t>
-  </si>
-  <si>
     <t>* payload 1</t>
   </si>
   <si>
@@ -378,12 +372,6 @@
     <t>* payload 20</t>
   </si>
   <si>
-    <t>* payload 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Last payload is Control Word From User</t>
-  </si>
-  <si>
     <t>* payload[2] =</t>
   </si>
   <si>
@@ -441,9 +429,6 @@
     <t>* payload[20] =</t>
   </si>
   <si>
-    <t xml:space="preserve"> "ESP8266 Client", #define PUB_TOPIC   "Tank ESP", tank_esp_ , len=21</t>
-  </si>
-  <si>
     <t>/* payload[0] =</t>
   </si>
   <si>
@@ -510,9 +495,6 @@
     <t xml:space="preserve"> 43floatState;  //byte34-float4;byte123-float3</t>
   </si>
   <si>
-    <t xml:space="preserve"> "ESP8266 ClientFlow", #define PUB_TOPIC   "Flow ESP", flow_esp_ , len=21</t>
-  </si>
-  <si>
     <t>Number of milliseconds in Time Window</t>
   </si>
   <si>
@@ -754,13 +736,86 @@
   </si>
   <si>
     <t>//Blynk.virtualWrite (V</t>
+  </si>
+  <si>
+    <t>/* payload 0</t>
+  </si>
+  <si>
+    <r>
+      <t>unsigned</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF9B2393"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>short</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF9B2393"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>#define  ESP_CLIENTID</t>
+  </si>
+  <si>
+    <t>#define FLO_CLIENTID</t>
+  </si>
+  <si>
+    <t>flow_data_payload[FLO_LEN] ;</t>
+  </si>
+  <si>
+    <t>data_payload[ESP_LEN] ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "ESP8266 ClientFlow", #define FLO_TOPIC   "Flow ESP", flow_esp_ , #define FLO_LEN 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "ESP8266 Client", #define ESP_TOPIC   "Tank ESP", tank_esp_ , #define ESP_LEN 21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -808,6 +863,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9B2393"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -916,7 +984,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2953,7 +3021,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3241,7 +3309,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3251,8 +3319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F5BC79-5CC4-4146-A4AC-12A07A1DA7E2}">
   <dimension ref="B3:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:E63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3269,274 +3337,274 @@
     <row r="3" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D4" s="2" t="s">
-        <v>3</v>
+        <v>235</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>134</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D5" s="3" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D6" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D7" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D8" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D10" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D11" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D12" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D13" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D14" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D15" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D16" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D17" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D18" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D19" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D20" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D21" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D22" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D23" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D24" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D25" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.2">
@@ -3545,10 +3613,10 @@
       </c>
       <c r="E26" s="6"/>
       <c r="J26" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.2">
@@ -3557,24 +3625,24 @@
       </c>
       <c r="E27" s="6"/>
       <c r="J27" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K27" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D28" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="K28" s="6" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="29" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3583,26 +3651,26 @@
       </c>
       <c r="E29" s="7"/>
       <c r="J29" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.2">
       <c r="J30" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.2">
       <c r="J31" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.2">
@@ -3612,17 +3680,17 @@
       <c r="K32" s="6"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="C33" s="11">
+      <c r="B33" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C33" s="10">
         <v>0</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>237</v>
+      <c r="D33" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>231</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>0</v>
@@ -3630,37 +3698,37 @@
       <c r="K33" s="6"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C34" s="11">
+      <c r="B34" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" s="10">
         <v>1</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>176</v>
+      <c r="D34" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>170</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C35" s="11">
+      <c r="B35" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C35" s="10">
         <v>2</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>177</v>
+      <c r="D35" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>1</v>
@@ -3668,527 +3736,527 @@
       <c r="K35" s="7"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C36" s="11">
+      <c r="B36" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C36" s="10">
         <v>3</v>
       </c>
-      <c r="D36" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>178</v>
+      <c r="D36" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C37" s="10">
         <v>4</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E37" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" s="10">
+        <v>5</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C38" s="11">
-        <v>5</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>193</v>
-      </c>
       <c r="E38" s="10" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C39" s="11">
+      <c r="B39" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C39" s="10">
         <v>6</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>194</v>
+      <c r="D39" s="10" t="s">
+        <v>188</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C40" s="11">
+      <c r="B40" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C40" s="10">
         <v>7</v>
       </c>
-      <c r="D40" s="11" t="s">
-        <v>195</v>
+      <c r="D40" s="10" t="s">
+        <v>189</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C41" s="10">
         <v>8</v>
       </c>
       <c r="D41" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B42" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C42" s="10">
+        <v>9</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B43" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C43" s="10">
+        <v>10</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B44" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C44" s="10">
+        <v>11</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B45" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C45" s="10">
+        <v>12</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B46" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C46" s="10">
+        <v>13</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B47" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C47" s="10">
+        <v>14</v>
+      </c>
+      <c r="D47" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="E41" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C42" s="11">
-        <v>9</v>
-      </c>
-      <c r="D42" s="11" t="s">
+      <c r="E47" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B48" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="10">
+        <v>15</v>
+      </c>
+      <c r="D48" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K42" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B43" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C43" s="11">
-        <v>10</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B44" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C44" s="11">
-        <v>11</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="J44" s="3" t="s">
+      <c r="E48" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="J48" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="K44" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C45" s="11">
-        <v>12</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C46" s="11">
-        <v>13</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B47" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C47" s="11">
-        <v>14</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="K47" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B48" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C48" s="11">
-        <v>15</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="K48" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B49" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C49" s="10">
         <v>16</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B50" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C50" s="10">
         <v>17</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B51" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C51" s="10">
         <v>18</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B52" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C52" s="10">
         <v>19</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B53" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C53" s="10">
         <v>20</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B54" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C54" s="10">
         <v>21</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C55" s="10">
         <v>22</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B56" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C56" s="10">
         <v>23</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B57" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C57" s="10">
         <v>24</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B58" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C58" s="10">
         <v>25</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B59" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C59" s="10">
         <v>26</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B60" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C60" s="10">
         <v>27</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B61" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C61" s="10">
         <v>28</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B62" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C62" s="10">
         <v>29</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B63" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C63" s="10">
         <v>30</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="J63" s="3" t="s">
         <v>1</v>
@@ -4207,24 +4275,24 @@
     </row>
     <row r="66" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D66" s="2" t="s">
-        <v>3</v>
+        <v>236</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D67" s="3" t="s">
-        <v>92</v>
+        <v>233</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>1</v>
@@ -4233,252 +4301,252 @@
     </row>
     <row r="68" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D68" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D69" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D70" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D71" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D72" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D73" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D74" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K74" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D75" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D76" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K76" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D77" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D78" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="K78" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D79" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="80" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D80" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D81" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D82" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D83" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D84" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D85" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D86" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="87" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D87" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="88" spans="4:11" x14ac:dyDescent="0.2">
@@ -4487,10 +4555,10 @@
       </c>
       <c r="E88" s="6"/>
       <c r="J88" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="4:11" x14ac:dyDescent="0.2">
@@ -4499,24 +4567,24 @@
       </c>
       <c r="E89" s="6"/>
       <c r="J89" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D90" s="3" t="s">
-        <v>113</v>
+      <c r="D90" s="11" t="s">
+        <v>234</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>114</v>
+        <v>237</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4525,34 +4593,34 @@
       </c>
       <c r="E91" s="7"/>
       <c r="J91" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="4:11" x14ac:dyDescent="0.2">
       <c r="J92" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K92" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="4:11" x14ac:dyDescent="0.2">
       <c r="J93" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K93" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="4:11" x14ac:dyDescent="0.2">
       <c r="J94" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K94" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" spans="4:11" x14ac:dyDescent="0.2">
@@ -4573,10 +4641,10 @@
     </row>
     <row r="98" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J98" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="K98" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="99" spans="10:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4588,178 +4656,178 @@
     <row r="106" spans="10:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="107" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J107" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K107" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="K107" s="5" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="108" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J108" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K108" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="109" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J109" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K109" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="110" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J110" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K110" s="6" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="111" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J111" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K111" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="112" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J112" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="K112" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="113" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J113" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K113" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="114" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J114" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K114" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="115" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J115" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K115" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="116" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J116" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K116" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="117" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J117" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K117" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="118" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J118" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K118" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="119" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J119" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K119" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="120" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J120" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K120" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="121" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J121" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K121" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="122" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J122" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K122" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="123" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J123" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K123" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="124" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J124" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K124" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="125" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J125" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K125" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="126" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J126" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K126" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="127" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J127" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K127" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="128" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J128" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K128" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="129" spans="10:11" x14ac:dyDescent="0.2">
@@ -4780,10 +4848,10 @@
     </row>
     <row r="132" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J132" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K132" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="133" spans="10:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4815,210 +4883,210 @@
   <sheetData>
     <row r="5" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
         <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
         <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
         <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
         <v>42</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
         <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
         <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
         <v>48</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
         <v>50</v>
-      </c>
-      <c r="F12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
         <v>52</v>
-      </c>
-      <c r="F13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
         <v>54</v>
-      </c>
-      <c r="F14" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" t="s">
         <v>56</v>
-      </c>
-      <c r="F15" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" t="s">
         <v>58</v>
-      </c>
-      <c r="F16" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E17" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
         <v>60</v>
-      </c>
-      <c r="F17" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E18" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" t="s">
         <v>62</v>
-      </c>
-      <c r="F18" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" t="s">
         <v>64</v>
-      </c>
-      <c r="F19" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E20" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" t="s">
         <v>66</v>
-      </c>
-      <c r="F20" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
         <v>68</v>
-      </c>
-      <c r="F21" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E22" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" t="s">
         <v>70</v>
-      </c>
-      <c r="F22" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="23" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" t="s">
         <v>72</v>
-      </c>
-      <c r="F23" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E24" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" t="s">
         <v>74</v>
-      </c>
-      <c r="F24" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="25" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" t="s">
         <v>76</v>
-      </c>
-      <c r="F25" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="26" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" t="s">
         <v>78</v>
-      </c>
-      <c r="F26" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="27" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E27" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" t="s">
         <v>80</v>
-      </c>
-      <c r="F27" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="28" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E28" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" t="s">
         <v>82</v>
-      </c>
-      <c r="F28" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="29" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E29" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" t="s">
         <v>84</v>
-      </c>
-      <c r="F29" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="30" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E30" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" t="s">
         <v>86</v>
-      </c>
-      <c r="F30" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Watchdog and MQTT prod vs dev
</commit_message>
<xml_diff>
--- a/WaterDiag.xlsx
+++ b/WaterDiag.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dub/Code/MilanoWaterProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3143B8D9-AA9E-2F4B-BAED-3B22CA77B4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460F13E6-9963-0041-887C-FD1B96B8CD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18940" yWindow="1180" windowWidth="46700" windowHeight="19020" activeTab="1" xr2:uid="{60223CC9-929C-2C40-9DF4-4D5E66E85102}"/>
+    <workbookView xWindow="1440" yWindow="500" windowWidth="46700" windowHeight="19020" activeTab="1" xr2:uid="{60223CC9-929C-2C40-9DF4-4D5E66E85102}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
     <sheet name="Future" sheetId="3" r:id="rId2"/>
-    <sheet name="Alerts" sheetId="4" r:id="rId3"/>
-    <sheet name="TestStruct" sheetId="5" r:id="rId4"/>
+    <sheet name="Calculations" sheetId="6" r:id="rId3"/>
+    <sheet name="Alerts" sheetId="4" r:id="rId4"/>
+    <sheet name="TestStruct" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="533">
   <si>
     <t>/*</t>
   </si>
@@ -1653,12 +1654,48 @@
   <si>
     <t xml:space="preserve"> Cycle Counter</t>
   </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>LSB</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Height of Water</t>
+  </si>
+  <si>
+    <t>Pi</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>VoltoGal</t>
+  </si>
+  <si>
+    <t>Gallons in Tank</t>
+  </si>
+  <si>
+    <t>Height in Ft</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1769,6 +1806,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1913,7 +1956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1974,6 +2017,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6633,7 +6678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F5BC79-5CC4-4146-A4AC-12A07A1DA7E2}">
   <dimension ref="B3:K133"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E67" sqref="E67:E87"/>
     </sheetView>
   </sheetViews>
@@ -8189,8 +8234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03884E4-1121-FE49-8CFC-397DF0F5A368}">
   <dimension ref="A1:R163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11794,6 +11839,203 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E1C9A1-DABD-5748-A871-466FBF261D9F}">
+  <dimension ref="B2:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="7" width="14.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>521</v>
+      </c>
+      <c r="C2" t="s">
+        <v>522</v>
+      </c>
+      <c r="D2" t="s">
+        <v>523</v>
+      </c>
+      <c r="E2" t="s">
+        <v>524</v>
+      </c>
+      <c r="F2" t="s">
+        <v>525</v>
+      </c>
+      <c r="G2" t="s">
+        <v>530</v>
+      </c>
+      <c r="H2" t="s">
+        <v>526</v>
+      </c>
+      <c r="I2" t="s">
+        <v>527</v>
+      </c>
+      <c r="J2" t="s">
+        <v>531</v>
+      </c>
+      <c r="K2" t="s">
+        <v>528</v>
+      </c>
+      <c r="L2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>135</v>
+      </c>
+      <c r="C3">
+        <f>HEX2DEC(B3)</f>
+        <v>309</v>
+      </c>
+      <c r="D3" s="32">
+        <v>3.2258064499999998E-3</v>
+      </c>
+      <c r="E3">
+        <f>D3*C3</f>
+        <v>0.99677419304999992</v>
+      </c>
+      <c r="F3">
+        <v>76.5</v>
+      </c>
+      <c r="G3">
+        <f>F3/12</f>
+        <v>6.375</v>
+      </c>
+      <c r="H3">
+        <v>3.1419000000000001</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <f>(I3*I3)*H3</f>
+        <v>50.270400000000002</v>
+      </c>
+      <c r="K3">
+        <f>(G3*J3)*7.048052</f>
+        <v>2258.7160070376003</v>
+      </c>
+      <c r="L3" s="33">
+        <f>K3</f>
+        <v>2258.7160070376003</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>117</v>
+      </c>
+      <c r="C4">
+        <f>HEX2DEC(B4)</f>
+        <v>279</v>
+      </c>
+      <c r="D4" s="32">
+        <v>3.2258064499999998E-3</v>
+      </c>
+      <c r="E4">
+        <f>D4*C4</f>
+        <v>0.89999999954999998</v>
+      </c>
+      <c r="F4">
+        <v>66.5</v>
+      </c>
+      <c r="G4">
+        <f>F4/12</f>
+        <v>5.541666666666667</v>
+      </c>
+      <c r="H4">
+        <v>3.1419000000000001</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <f>(I4*I4)*H4</f>
+        <v>50.270400000000002</v>
+      </c>
+      <c r="K4">
+        <f>(G4*J4)*7.048052</f>
+        <v>1963.4590126536004</v>
+      </c>
+      <c r="L4" s="33">
+        <f>K4</f>
+        <v>1963.4590126536004</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>417</v>
+      </c>
+      <c r="L8" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>0.99677419304999992</v>
+      </c>
+      <c r="F9">
+        <v>76.5</v>
+      </c>
+      <c r="G9">
+        <v>6.375</v>
+      </c>
+      <c r="H9">
+        <v>3.1419000000000001</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>50.270400000000002</v>
+      </c>
+      <c r="K9">
+        <v>2258.7160070376003</v>
+      </c>
+      <c r="L9">
+        <v>2258.7160070376003</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>0.89999999954999998</v>
+      </c>
+      <c r="F10">
+        <v>66.5</v>
+      </c>
+      <c r="G10">
+        <v>5.541666666666667</v>
+      </c>
+      <c r="H10">
+        <v>3.1419000000000001</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>50.270400000000002</v>
+      </c>
+      <c r="K10">
+        <v>1963.4590126536004</v>
+      </c>
+      <c r="L10">
+        <v>1963.4590126536004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EF0447-FEAA-DE4B-B6F4-489E40F1B706}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -12236,7 +12478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE230EF6-CC67-FC4F-BD53-EEEF0DC38F92}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>

</xml_diff>

<commit_message>
added code to check for Prod Server or Dev Server & JSON
</commit_message>
<xml_diff>
--- a/WaterDiag.xlsx
+++ b/WaterDiag.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dub/Code/MilanoWaterProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460F13E6-9963-0041-887C-FD1B96B8CD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C31A93-FDF4-244D-A059-C6F3C802DDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="500" windowWidth="46700" windowHeight="19020" activeTab="1" xr2:uid="{60223CC9-929C-2C40-9DF4-4D5E66E85102}"/>
   </bookViews>
@@ -18,7 +18,11 @@
     <sheet name="Calculations" sheetId="6" r:id="rId3"/>
     <sheet name="Alerts" sheetId="4" r:id="rId4"/>
     <sheet name="TestStruct" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet2!$A$1:$B$142</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="539">
   <si>
     <t>/*</t>
   </si>
@@ -1690,12 +1694,30 @@
   <si>
     <t>y</t>
   </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>Avg Sensor Value</t>
+  </si>
+  <si>
+    <t>WaterHeight = ((PresSensorValue - ConstantX) / Constant) + .1</t>
+  </si>
+  <si>
+    <t>ConstantX</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1810,6 +1832,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FFB5CEA8"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -1956,7 +1984,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2019,6 +2047,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2034,6 +2063,2326 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$1:$A$141</c:f>
+              <c:strCache>
+                <c:ptCount val="141"/>
+                <c:pt idx="0">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>&gt;</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>|</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>Avg Sensor Value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$141</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="141"/>
+                <c:pt idx="0">
+                  <c:v>0.93951600000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94032300000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94064499999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94128999999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.941774</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.94225800000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.942581</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.94274199999999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94241900000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.94161300000000003</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.94080600000000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.94064499999999995</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.94016100000000002</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.93983899999999998</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.94064499999999995</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.94112899999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.94161300000000003</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.94257999999999997</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.94306400000000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.94322600000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.94306400000000001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.94338699999999998</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.94338699999999998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.94290300000000005</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.94209699999999996</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.94145100000000004</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.94096800000000003</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.94048399999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.94048399999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.94016100000000002</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.93983899999999998</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.93983899999999998</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.94032199999999999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.94048399999999999</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.94064499999999995</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.94064499999999995</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.94016100000000002</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.93967699999999998</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.93935500000000005</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.93903199999999998</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.93838699999999997</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.93774199999999996</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.937581</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.937581</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.937419</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.93725800000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0DE5-F944-9B55-A11B9BCB3037}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1039572383"/>
+        <c:axId val="1022591472"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1039572383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1022591472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1022591472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1039572383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$Y$79:$Y$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$Z$79:$Z$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2258</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2058</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-97C4-6844-B272-B41E32006ECC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="390906032"/>
+        <c:axId val="390886224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="390906032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390886224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="390886224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="390906032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6376,6 +8725,83 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7079DE55-B4A0-8863-4DFD-C26F9F87424F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B837EC13-52A7-3C8E-FFEB-44B76D730010}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8234,8 +10660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03884E4-1121-FE49-8CFC-397DF0F5A368}">
   <dimension ref="A1:R163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13053,4 +15479,1225 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227A706B-9ECB-5744-BC59-C11D58CA612E}">
+  <dimension ref="A1:AC141"/>
+  <sheetViews>
+    <sheetView topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="V113" sqref="V113:V121"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B1">
+        <v>0.93951600000000002</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>535</v>
+      </c>
+      <c r="B4">
+        <v>0.94032300000000002</v>
+      </c>
+      <c r="C4">
+        <f>B1-B4</f>
+        <v>-8.0700000000000216E-4</v>
+      </c>
+      <c r="E4">
+        <v>0.93951600000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>533</v>
+      </c>
+      <c r="E5">
+        <v>0.94032300000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>534</v>
+      </c>
+      <c r="E6">
+        <v>0.94064499999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>535</v>
+      </c>
+      <c r="B7">
+        <v>0.94064499999999995</v>
+      </c>
+      <c r="C7">
+        <f>B4-B7</f>
+        <v>-3.2199999999993345E-4</v>
+      </c>
+      <c r="E7">
+        <v>0.94128999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>533</v>
+      </c>
+      <c r="E8">
+        <v>0.941774</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>534</v>
+      </c>
+      <c r="E9">
+        <v>0.94225800000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>535</v>
+      </c>
+      <c r="B10">
+        <v>0.94128999999999996</v>
+      </c>
+      <c r="C10">
+        <f>B7-B10</f>
+        <v>-6.4500000000000668E-4</v>
+      </c>
+      <c r="E10">
+        <v>0.942581</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>533</v>
+      </c>
+      <c r="E11">
+        <v>0.94274199999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>534</v>
+      </c>
+      <c r="E12">
+        <v>0.94241900000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>535</v>
+      </c>
+      <c r="B13">
+        <v>0.941774</v>
+      </c>
+      <c r="C13">
+        <f>B10-B13</f>
+        <v>-4.8400000000003995E-4</v>
+      </c>
+      <c r="E13">
+        <v>0.94161300000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>533</v>
+      </c>
+      <c r="E14">
+        <v>0.94080600000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>534</v>
+      </c>
+      <c r="E15">
+        <v>0.94064499999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>535</v>
+      </c>
+      <c r="B16">
+        <v>0.94225800000000004</v>
+      </c>
+      <c r="C16">
+        <f>B13-B16</f>
+        <v>-4.8400000000003995E-4</v>
+      </c>
+      <c r="E16">
+        <v>0.94016100000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>533</v>
+      </c>
+      <c r="E17">
+        <v>0.93983899999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>534</v>
+      </c>
+      <c r="E18">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>535</v>
+      </c>
+      <c r="B19">
+        <v>0.942581</v>
+      </c>
+      <c r="C19">
+        <f>B16-B19</f>
+        <v>-3.2299999999996221E-4</v>
+      </c>
+      <c r="E19">
+        <v>0.94064499999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>533</v>
+      </c>
+      <c r="E20">
+        <v>0.94112899999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>534</v>
+      </c>
+      <c r="E21">
+        <v>0.94161300000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>535</v>
+      </c>
+      <c r="B22">
+        <v>0.94274199999999997</v>
+      </c>
+      <c r="C22">
+        <f>B19-B22</f>
+        <v>-1.6099999999996673E-4</v>
+      </c>
+      <c r="E22">
+        <v>0.94257999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>533</v>
+      </c>
+      <c r="E23">
+        <v>0.94306400000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>534</v>
+      </c>
+      <c r="E24">
+        <v>0.94322600000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>535</v>
+      </c>
+      <c r="B25">
+        <v>0.94241900000000001</v>
+      </c>
+      <c r="C25">
+        <f>B22-B25</f>
+        <v>3.2299999999996221E-4</v>
+      </c>
+      <c r="E25">
+        <v>0.94306400000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>533</v>
+      </c>
+      <c r="E26">
+        <v>0.94338699999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>534</v>
+      </c>
+      <c r="E27">
+        <v>0.94338699999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>535</v>
+      </c>
+      <c r="B28">
+        <v>0.94161300000000003</v>
+      </c>
+      <c r="C28">
+        <f>B25-B28</f>
+        <v>8.059999999999734E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>535</v>
+      </c>
+      <c r="B31">
+        <v>0.94080600000000003</v>
+      </c>
+      <c r="C31">
+        <f>B28-B31</f>
+        <v>8.0700000000000216E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>535</v>
+      </c>
+      <c r="B34">
+        <v>0.94064499999999995</v>
+      </c>
+      <c r="C34">
+        <f>B31-B34</f>
+        <v>1.6100000000007775E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>535</v>
+      </c>
+      <c r="B37">
+        <v>0.94016100000000002</v>
+      </c>
+      <c r="C37">
+        <f>B34-B37</f>
+        <v>4.8399999999992893E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>535</v>
+      </c>
+      <c r="B40">
+        <v>0.93983899999999998</v>
+      </c>
+      <c r="C40">
+        <f>B37-B40</f>
+        <v>3.2200000000004447E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>535</v>
+      </c>
+      <c r="B43">
+        <v>0.94</v>
+      </c>
+      <c r="C43">
+        <f>B40-B43</f>
+        <v>-1.6099999999996673E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>535</v>
+      </c>
+      <c r="B46">
+        <v>0.94064499999999995</v>
+      </c>
+      <c r="C46">
+        <f>B43-B46</f>
+        <v>-6.4500000000000668E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>535</v>
+      </c>
+      <c r="B49">
+        <v>0.94112899999999999</v>
+      </c>
+      <c r="C49">
+        <f>B46-B49</f>
+        <v>-4.8400000000003995E-4</v>
+      </c>
+      <c r="AA49">
+        <f>AB49*Z61</f>
+        <v>0.98064516129032253</v>
+      </c>
+      <c r="AB49">
+        <f>HEX2DEC(AC49)</f>
+        <v>304</v>
+      </c>
+      <c r="AC49">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>535</v>
+      </c>
+      <c r="B52">
+        <v>0.94161300000000003</v>
+      </c>
+      <c r="C52">
+        <f>B49-B52</f>
+        <v>-4.8400000000003995E-4</v>
+      </c>
+      <c r="AA52">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="AB52">
+        <f>AA52/Z61</f>
+        <v>305.65999999999997</v>
+      </c>
+      <c r="AC52" t="str">
+        <f>DEC2HEX(AB52)</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>535</v>
+      </c>
+      <c r="B55">
+        <v>0.94257999999999997</v>
+      </c>
+      <c r="C55">
+        <f>B52-B55</f>
+        <v>-9.6699999999994013E-4</v>
+      </c>
+      <c r="AA55">
+        <f>AB55*Z61</f>
+        <v>0.98709677419354835</v>
+      </c>
+      <c r="AB55">
+        <f>HEX2DEC(AC55)</f>
+        <v>306</v>
+      </c>
+      <c r="AC55">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>535</v>
+      </c>
+      <c r="B58">
+        <v>0.94306400000000001</v>
+      </c>
+      <c r="C58">
+        <f>B55-B58</f>
+        <v>-4.8400000000003995E-4</v>
+      </c>
+      <c r="AA58">
+        <f>AB58*Z61</f>
+        <v>0.99032258064516132</v>
+      </c>
+      <c r="AB58">
+        <f>HEX2DEC(AC58)</f>
+        <v>307</v>
+      </c>
+      <c r="AC58">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>535</v>
+      </c>
+      <c r="B61">
+        <v>0.94322600000000001</v>
+      </c>
+      <c r="C61">
+        <f>B58-B61</f>
+        <v>-1.6199999999999548E-4</v>
+      </c>
+      <c r="X61">
+        <v>3.3</v>
+      </c>
+      <c r="Y61">
+        <v>1023</v>
+      </c>
+      <c r="Z61">
+        <f>X61/Y61</f>
+        <v>3.2258064516129032E-3</v>
+      </c>
+      <c r="AA61">
+        <f>AB61*Z67</f>
+        <v>0</v>
+      </c>
+      <c r="AB61">
+        <f>HEX2DEC(AC61)</f>
+        <v>308</v>
+      </c>
+      <c r="AC61">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>535</v>
+      </c>
+      <c r="B64">
+        <v>0.94306400000000001</v>
+      </c>
+      <c r="C64">
+        <f>B61-B64</f>
+        <v>1.6199999999999548E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>535</v>
+      </c>
+      <c r="B67">
+        <v>0.94338699999999998</v>
+      </c>
+      <c r="C67">
+        <f>B64-B67</f>
+        <v>-3.2299999999996221E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>535</v>
+      </c>
+      <c r="B70">
+        <v>0.94338699999999998</v>
+      </c>
+      <c r="C70">
+        <f>B67-B70</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>535</v>
+      </c>
+      <c r="B73">
+        <v>0.94290300000000005</v>
+      </c>
+      <c r="C73">
+        <f>B70-B73</f>
+        <v>4.8399999999992893E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>535</v>
+      </c>
+      <c r="B76">
+        <v>0.94209699999999996</v>
+      </c>
+      <c r="C76">
+        <f>B73-B76</f>
+        <v>8.0600000000008443E-4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>535</v>
+      </c>
+      <c r="B79">
+        <v>0.94145100000000004</v>
+      </c>
+      <c r="C79">
+        <f>B76-B79</f>
+        <v>6.4599999999992441E-4</v>
+      </c>
+      <c r="Y79">
+        <v>2.4</v>
+      </c>
+      <c r="Z79">
+        <v>2258</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>535</v>
+      </c>
+      <c r="B82">
+        <v>0.94096800000000003</v>
+      </c>
+      <c r="C82">
+        <f>B79-B82</f>
+        <v>4.830000000000112E-4</v>
+      </c>
+      <c r="Y82">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Z82">
+        <v>2058</v>
+      </c>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>535</v>
+      </c>
+      <c r="B85">
+        <v>0.94048399999999999</v>
+      </c>
+      <c r="C85">
+        <f>B82-B85</f>
+        <v>4.8400000000003995E-4</v>
+      </c>
+      <c r="Y85">
+        <v>2</v>
+      </c>
+      <c r="Z85">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>535</v>
+      </c>
+      <c r="B88">
+        <v>0.94048399999999999</v>
+      </c>
+      <c r="C88">
+        <f>B85-B88</f>
+        <v>0</v>
+      </c>
+      <c r="Y88">
+        <v>1.8</v>
+      </c>
+      <c r="Z88">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>535</v>
+      </c>
+      <c r="B91">
+        <v>0.94016100000000002</v>
+      </c>
+      <c r="C91">
+        <f>B88-B91</f>
+        <v>3.2299999999996221E-4</v>
+      </c>
+      <c r="Y91">
+        <v>1.6</v>
+      </c>
+      <c r="Z91">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>535</v>
+      </c>
+      <c r="B93">
+        <v>0.93983899999999998</v>
+      </c>
+      <c r="C93">
+        <f>B90-B93</f>
+        <v>-0.93983899999999998</v>
+      </c>
+      <c r="Y93">
+        <v>1.4</v>
+      </c>
+      <c r="Z93">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>535</v>
+      </c>
+      <c r="B96">
+        <v>0.93983899999999998</v>
+      </c>
+      <c r="C96">
+        <f>B93-B96</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>535</v>
+      </c>
+      <c r="B99">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>535</v>
+      </c>
+      <c r="B102">
+        <v>0.94032199999999999</v>
+      </c>
+      <c r="V102" t="s">
+        <v>537</v>
+      </c>
+      <c r="W102">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>535</v>
+      </c>
+      <c r="B105">
+        <v>0.94048399999999999</v>
+      </c>
+      <c r="V105" t="s">
+        <v>538</v>
+      </c>
+      <c r="W105">
+        <v>9.6199999999999994E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>535</v>
+      </c>
+      <c r="B108">
+        <v>0.94064499999999995</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>535</v>
+      </c>
+      <c r="B111">
+        <v>0.94064499999999995</v>
+      </c>
+      <c r="V111" s="34" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="113" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>535</v>
+      </c>
+      <c r="B113">
+        <v>0.94016100000000002</v>
+      </c>
+      <c r="V113">
+        <f>((E4-$W$102)/$W$105)+0.1</f>
+        <v>6.3319750519750517</v>
+      </c>
+    </row>
+    <row r="114" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>533</v>
+      </c>
+      <c r="V114">
+        <f t="shared" ref="V114:V121" si="0">((E5-$W$102)/$W$105)+0.1</f>
+        <v>6.3403638253638244</v>
+      </c>
+    </row>
+    <row r="115" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>534</v>
+      </c>
+      <c r="V115">
+        <f t="shared" si="0"/>
+        <v>6.3437110187110175</v>
+      </c>
+    </row>
+    <row r="116" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>534</v>
+      </c>
+      <c r="V116">
+        <f t="shared" si="0"/>
+        <v>6.3504158004157993</v>
+      </c>
+    </row>
+    <row r="117" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>535</v>
+      </c>
+      <c r="B117">
+        <v>0.93967699999999998</v>
+      </c>
+      <c r="V117">
+        <f t="shared" si="0"/>
+        <v>6.3554469854469859</v>
+      </c>
+    </row>
+    <row r="118" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>534</v>
+      </c>
+      <c r="V118">
+        <f t="shared" si="0"/>
+        <v>6.3604781704781699</v>
+      </c>
+    </row>
+    <row r="119" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>533</v>
+      </c>
+      <c r="V119">
+        <f t="shared" si="0"/>
+        <v>6.3638357588357595</v>
+      </c>
+    </row>
+    <row r="120" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>535</v>
+      </c>
+      <c r="B120">
+        <v>0.93935500000000005</v>
+      </c>
+      <c r="V120">
+        <f t="shared" si="0"/>
+        <v>6.3655093555093547</v>
+      </c>
+    </row>
+    <row r="121" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>534</v>
+      </c>
+      <c r="V121">
+        <f t="shared" si="0"/>
+        <v>6.3621517671517678</v>
+      </c>
+    </row>
+    <row r="122" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="123" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>535</v>
+      </c>
+      <c r="B123">
+        <v>0.93903199999999998</v>
+      </c>
+    </row>
+    <row r="124" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="125" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="126" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>535</v>
+      </c>
+      <c r="B126">
+        <v>0.93838699999999997</v>
+      </c>
+    </row>
+    <row r="127" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="128" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>535</v>
+      </c>
+      <c r="B129">
+        <v>0.93774199999999996</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>535</v>
+      </c>
+      <c r="B132">
+        <v>0.937581</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>535</v>
+      </c>
+      <c r="B135">
+        <v>0.937581</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>535</v>
+      </c>
+      <c r="B138">
+        <v>0.937419</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>535</v>
+      </c>
+      <c r="B141">
+        <v>0.93725800000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B142" xr:uid="{227A706B-9ECB-5744-BC59-C11D58CA612E}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added Sparkfun Thing Dev board to flow sensor
</commit_message>
<xml_diff>
--- a/WaterDiag.xlsx
+++ b/WaterDiag.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dub/Code/MilanoWaterProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B3C71B5-2A0E-6F4A-B534-9FCF888D4226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63748BEA-E918-9241-8C75-42DB357C82EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="1160" windowWidth="46700" windowHeight="19020" activeTab="1" xr2:uid="{60223CC9-929C-2C40-9DF4-4D5E66E85102}"/>
+    <workbookView xWindow="2460" yWindow="500" windowWidth="46700" windowHeight="19020" activeTab="1" xr2:uid="{60223CC9-929C-2C40-9DF4-4D5E66E85102}"/>
   </bookViews>
   <sheets>
     <sheet name="Previous" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="TestStruct" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
     <sheet name="FlowCalc" sheetId="8" r:id="rId7"/>
-    <sheet name="PressCalc" sheetId="9" r:id="rId8"/>
+    <sheet name="Chart1" sheetId="10" r:id="rId8"/>
+    <sheet name="PressCalc" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">FlowCalc!$A$79:$AF$567</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3464" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3476" uniqueCount="781">
   <si>
     <t>/*</t>
   </si>
@@ -2395,6 +2396,51 @@
   </si>
   <si>
     <t>tankgal_data_payload[TANKGAL_LEN] ;</t>
+  </si>
+  <si>
+    <t>Water Height Press</t>
+  </si>
+  <si>
+    <t>Water Height Ultra</t>
+  </si>
+  <si>
+    <t>Tank Temperature</t>
+  </si>
+  <si>
+    <t>Tank Humidity</t>
+  </si>
+  <si>
+    <t>inches of water</t>
+  </si>
+  <si>
+    <t>feet</t>
+  </si>
+  <si>
+    <t>volume cu/ft</t>
+  </si>
+  <si>
+    <t>gallons</t>
+  </si>
+  <si>
+    <t>CM from Ultrasond</t>
+  </si>
+  <si>
+    <t>Height of Water Ultra</t>
+  </si>
+  <si>
+    <t>raw sensor</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Feet</t>
+  </si>
+  <si>
+    <t>SenorVal</t>
+  </si>
+  <si>
+    <t>scaled</t>
   </si>
 </sst>
 </file>
@@ -2532,7 +2578,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2596,6 +2642,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2680,7 +2732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2751,6 +2803,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3111,7 +3164,421 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PressCalc!$U$22:$AB$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.5709677411499998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6645161281999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8193548378</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9516129022499999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0580645155999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1548387090999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2516129026</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.354838709</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PressCalc!$U$23:$AB$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.5833333333333335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.208333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.885416666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8229166666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2604166666666665</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1373-DC40-AC77-7D77E8CB1987}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="754043792"/>
+        <c:axId val="754812768"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="754043792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="754812768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="754812768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="754043792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3665,6 +4132,533 @@
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E8DCA7A8-BAAC-7645-97C5-749345EB628D}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="146" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8179,6 +9173,39 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8672534" cy="6280411"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2999FBA3-87D4-DA5E-D4EB-25938CDBBC9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10034,8 +11061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03884E4-1121-FE49-8CFC-397DF0F5A368}">
   <dimension ref="A4:R191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10623,7 +11650,7 @@
       <c r="D42" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="42" t="s">
         <v>197</v>
       </c>
       <c r="J42" s="3" t="s">
@@ -10655,7 +11682,7 @@
       <c r="D43" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="42" t="s">
         <v>441</v>
       </c>
       <c r="J43" s="3" t="s">
@@ -10687,14 +11714,14 @@
       <c r="D44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="42" t="s">
         <v>442</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>70</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>13</v>
+        <v>766</v>
       </c>
       <c r="M44" t="s">
         <v>87</v>
@@ -10719,14 +11746,14 @@
       <c r="D45" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="42" t="s">
         <v>443</v>
       </c>
       <c r="J45" s="3" t="s">
         <v>71</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>13</v>
+        <v>767</v>
       </c>
       <c r="M45" t="s">
         <v>87</v>
@@ -10751,14 +11778,14 @@
       <c r="D46" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="42" t="s">
         <v>444</v>
       </c>
       <c r="J46" s="3" t="s">
         <v>72</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>13</v>
+        <v>768</v>
       </c>
       <c r="M46" t="s">
         <v>87</v>
@@ -10790,7 +11817,7 @@
         <v>73</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>13</v>
+        <v>769</v>
       </c>
       <c r="M47" t="s">
         <v>87</v>
@@ -12144,7 +13171,7 @@
       <c r="D104" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E104" s="6" t="s">
+      <c r="E104" s="42" t="s">
         <v>111</v>
       </c>
       <c r="J104" s="3" t="s">
@@ -15194,8 +16221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227A706B-9ECB-5744-BC59-C11D58CA612E}">
   <dimension ref="A1:AC141"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="W78" sqref="W78:X79"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="W107" sqref="W107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -55894,15 +56921,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749A8602-3B3D-E049-A50C-F77EAF1374E8}">
-  <dimension ref="B3:J18"/>
+  <dimension ref="B3:AB33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>338</v>
       </c>
@@ -55913,13 +56940,75 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B5">
         <f>(B3*C3)/D3</f>
         <v>32.977054500000001</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="O6" s="30">
+        <v>3.2258064499999998E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="O8" t="s">
+        <v>780</v>
+      </c>
+      <c r="P8" t="s">
+        <v>776</v>
+      </c>
+      <c r="R8" t="s">
+        <v>770</v>
+      </c>
+      <c r="T8" t="s">
+        <v>771</v>
+      </c>
+      <c r="V8" t="s">
+        <v>772</v>
+      </c>
+      <c r="X8" t="s">
+        <v>773</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>775</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="9" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <f t="shared" ref="O9:O16" si="0">P9*$O$6</f>
+        <v>1.0580645155999999</v>
+      </c>
+      <c r="P9">
+        <v>328</v>
+      </c>
+      <c r="R9">
+        <v>16</v>
+      </c>
+      <c r="T9">
+        <f t="shared" ref="T9:T16" si="1">R9/12</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="V9">
+        <f t="shared" ref="V9:V16" si="2">(16*PI())*T9</f>
+        <v>67.020643276582248</v>
+      </c>
+      <c r="X9">
+        <f t="shared" ref="X9:X16" si="3">V9*7.048052</f>
+        <v>472.36497888680208</v>
+      </c>
+      <c r="Z9">
+        <f>(6.3783+0.748)-AB9/30.48</f>
+        <v>1.3848301837270345</v>
+      </c>
+      <c r="AB9">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>3.3</v>
       </c>
@@ -55929,85 +57018,396 @@
       <c r="D10">
         <v>1023</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>1.1548387090999999</v>
+      </c>
+      <c r="P10">
+        <v>358</v>
+      </c>
+      <c r="R10">
+        <v>21.875</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>1.8229166666666667</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="2"/>
+        <v>91.629785729702306</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="3"/>
+        <v>645.81149457179981</v>
+      </c>
+      <c r="Z10">
+        <f>(6.3783+0.748)-AB10/30.48</f>
+        <v>2.9924417322834653</v>
+      </c>
+      <c r="AB10">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>1.2516129026</v>
+      </c>
+      <c r="P11">
+        <v>388</v>
+      </c>
+      <c r="R11">
+        <v>27.125</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>2.2604166666666665</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="2"/>
+        <v>113.62093430483084</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="3"/>
+        <v>800.80625326903169</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>1.354838709</v>
+      </c>
+      <c r="P12">
+        <v>420</v>
+      </c>
+      <c r="R12">
+        <v>33</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>2.75</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="2"/>
+        <v>138.23007675795088</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="3"/>
+        <v>974.25276895402931</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>1.5709677411499998</v>
+      </c>
+      <c r="P13">
+        <v>487</v>
+      </c>
+      <c r="R13">
+        <v>43</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>3.5833333333333335</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="2"/>
+        <v>180.1179788058148</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="3"/>
+        <v>1269.4808807582806</v>
+      </c>
+      <c r="Z13">
+        <f>(6.3783+0.748)-AB13/30.48</f>
+        <v>7.1263000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>742</v>
       </c>
-      <c r="G12">
+      <c r="G14">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>1.6645161281999998</v>
+      </c>
+      <c r="P14">
+        <v>516</v>
+      </c>
+      <c r="R14">
+        <v>50.5</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>4.208333333333333</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="2"/>
+        <v>211.53390534171271</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="3"/>
+        <v>1490.9019646114689</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>743</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <f>B10/D10</f>
         <v>3.2258064516129032E-3</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0.5</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>2.5</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>1.8193548378</v>
+      </c>
+      <c r="P15">
+        <v>564</v>
+      </c>
+      <c r="R15">
+        <v>58.625</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>4.885416666666667</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="2"/>
+        <v>245.56782575560217</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="3"/>
+        <v>1730.7748054524234</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>50</v>
       </c>
-      <c r="G14">
+      <c r="G16">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <f>B3*C13</f>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>1.9516129022499999</v>
+      </c>
+      <c r="P16">
+        <v>605</v>
+      </c>
+      <c r="R16">
+        <v>68</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="2"/>
+        <v>284.83773392547459</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="3"/>
+        <v>2007.5511602689091</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f>B3*C15</f>
         <v>1.0903225806451613</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>745</v>
       </c>
-      <c r="D15">
-        <f>J18</f>
+      <c r="D17">
+        <f>J20</f>
         <v>40.816326530612244</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <f>B15*D15</f>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f>B17*D17</f>
         <v>44.502962475312707</v>
       </c>
-      <c r="G17">
+      <c r="G19">
         <v>2.4500000000000002</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H19" t="s">
         <v>417</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I19" t="s">
         <v>744</v>
       </c>
-      <c r="J17">
+      <c r="J19">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H18" t="s">
+    <row r="20" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
         <v>417</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I20" t="s">
         <v>744</v>
       </c>
-      <c r="J18">
-        <f>J17/G17</f>
+      <c r="J20">
+        <f>J19/G19</f>
         <v>40.816326530612244</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="T22" t="s">
+        <v>779</v>
+      </c>
+      <c r="U22">
+        <f>R24*$O$6</f>
+        <v>1.5709677411499998</v>
+      </c>
+      <c r="V22">
+        <f>R25*$O$6</f>
+        <v>1.6645161281999998</v>
+      </c>
+      <c r="W22">
+        <f>R26*$O$6</f>
+        <v>1.8193548378</v>
+      </c>
+      <c r="X22">
+        <f>R27*$O$6</f>
+        <v>1.9516129022499999</v>
+      </c>
+      <c r="Y22">
+        <v>1.0580645155999999</v>
+      </c>
+      <c r="Z22">
+        <v>1.1548387090999999</v>
+      </c>
+      <c r="AA22">
+        <v>1.2516129026</v>
+      </c>
+      <c r="AB22">
+        <v>1.354838709</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="Q23" t="s">
+        <v>778</v>
+      </c>
+      <c r="R23" t="s">
+        <v>777</v>
+      </c>
+      <c r="T23" t="s">
+        <v>778</v>
+      </c>
+      <c r="U23">
+        <v>3.5833333333333335</v>
+      </c>
+      <c r="V23">
+        <v>4.208333333333333</v>
+      </c>
+      <c r="W23">
+        <v>4.885416666666667</v>
+      </c>
+      <c r="X23">
+        <v>5.666666666666667</v>
+      </c>
+      <c r="Y23">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="Z23">
+        <v>1.8229166666666667</v>
+      </c>
+      <c r="AA23">
+        <v>2.2604166666666665</v>
+      </c>
+      <c r="AB23">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="Q24">
+        <v>3.5833333333333335</v>
+      </c>
+      <c r="R24">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="Q25">
+        <v>4.208333333333333</v>
+      </c>
+      <c r="R25">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="Q26">
+        <v>4.885416666666667</v>
+      </c>
+      <c r="R26">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="Q27">
+        <v>5.666666666666667</v>
+      </c>
+      <c r="R27">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="O30">
+        <f>(5.3113*O13)-4.7174</f>
+        <v>3.6264809635699944</v>
+      </c>
+      <c r="Q30">
+        <f>(3.0242*O13)+0.1028</f>
+        <v>4.8537206427858299</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="O31">
+        <f>(5.3113*O14)-4.7174</f>
+        <v>4.1233445117086589</v>
+      </c>
+      <c r="Q31">
+        <f>(3.0242*O14)+0.1028</f>
+        <v>5.1366296749024398</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="O32">
+        <f>(5.3113*O15)-4.7174</f>
+        <v>4.9457393500071412</v>
+      </c>
+      <c r="Q32">
+        <f>(3.0242*O15)+0.1028</f>
+        <v>5.6048929004747601</v>
+      </c>
+    </row>
+    <row r="33" spans="15:17" x14ac:dyDescent="0.2">
+      <c r="O33">
+        <f>(5.3113*O16)-4.7174</f>
+        <v>5.6482016077204253</v>
+      </c>
+      <c r="Q33">
+        <f>(3.0242*O16)+0.1028</f>
+        <v>6.0048677389844505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>